<commit_message>
fix: add correct xlsx template
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-inscrit-sans-contrat-ft.xlsx
+++ b/server/static/mission-locale/modele-inscrit-sans-contrat-ft.xlsx
@@ -1,84 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D875191-4DCD-4002-9F88-3ECE6450F40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohann/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33DE8310-D124-184F-9CF3-8C72E4FDF046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
-    <sheet name="À traiter" sheetId="2" r:id="rId2"/>
+    <sheet name="A traiter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr dataExtractLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Le tableau de bord de l'apprentissage vous met à disposition les contacts de jeunes n'ayant pas de contrats.</t>
-  </si>
-  <si>
-    <t>Merci de ne pas diffuser ces listes.</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,12 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,7 +75,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -421,52 +371,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C19"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="3"/>
-    </row>
+    <row r="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="3" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="5" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="7" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="8" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="9" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="11" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="12" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="13" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="14" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="15" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="16" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="50" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: add correct xlsx template (#4468)
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-inscrit-sans-contrat-ft.xlsx
+++ b/server/static/mission-locale/modele-inscrit-sans-contrat-ft.xlsx
@@ -1,84 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D875191-4DCD-4002-9F88-3ECE6450F40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohann/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33DE8310-D124-184F-9CF3-8C72E4FDF046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
-    <sheet name="À traiter" sheetId="2" r:id="rId2"/>
+    <sheet name="A traiter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr dataExtractLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Le tableau de bord de l'apprentissage vous met à disposition les contacts de jeunes n'ayant pas de contrats.</t>
-  </si>
-  <si>
-    <t>Merci de ne pas diffuser ces listes.</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,12 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,7 +75,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -421,52 +371,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C19"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="3"/>
-    </row>
+    <row r="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="3" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="5" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="7" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="8" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="9" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="11" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="12" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="13" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="14" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="15" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="16" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="50" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>